<commit_message>
Stated filling out the readme; realized I hadn't been using the palace, so it was missing some features it was supposed to have; mnemonics now have windows, but they still don't have doors or staircases; will need to get on that soon. Also, while I was working on this, changed the way Mnemonics worked from a straight function call to hash function, so it should be a bit faster.
</commit_message>
<xml_diff>
--- a/Mnemonics.xlsx
+++ b/Mnemonics.xlsx
@@ -13,9 +13,10 @@
     <sheet name="People" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Actions" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Objects" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Verbs (Candidates)" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Objects (Candidates)" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Notes" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="People (Candidates)" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Action (Candidates)" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Objects (Candidates)" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Notes" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="570">
   <si>
     <t xml:space="preserve">Object</t>
   </si>
@@ -984,6 +985,78 @@
   </si>
   <si>
     <t xml:space="preserve">zebra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject (Candidates)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam, Abraham, Aaron, Abel, Appolyon, Azriel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baal, Beelzebub, Bathsheba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cain, Cyrus,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dagon, Daniel, Darius, Deborah, David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elijah, Enoch, Esther, Esau, Eve, Ezra, Ezekiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felix, Festus (Both Roman dudes in charge of Judea. :/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gideon, Goliath,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaac, Iscariot,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus, Judas, Jacob, James, Jehovah, Joseph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K (Wikipedia lists a lot of names, none of which I recognize)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leah, Luke, Lucifer, Lot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magdelene, Mathew, Mary, Michael, Moses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noah, Nimrod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obadiah (Prophet and descendent of Esau; everyone else is more obsure than this), Omar (obsure, but makes me think of Captain Omar)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul, Peter, Pharoah, Pharisees, Philistines, (Maybe one of these can work for our F?), Pilate,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queen of Sheba (Aparently the only names)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruth, Rachel,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seth, Samuel, Saul, Solomon, Samson, Simon, Sarah, Silas,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas, Timothy,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uzziah (King of Israel), Uriah (Husband of Bathsheba), Uriel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W (literally none)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X None in the Bible, but we might put in Xerxes and ignore the other persian kings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yahweh, Yubal, Yeshua,</t>
   </si>
   <si>
     <t xml:space="preserve">Attack</t>
@@ -1674,7 +1747,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1717,19 +1790,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -1788,7 +1848,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1813,7 +1873,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1821,23 +1881,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2942,7 +2990,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2956,6 +3004,9 @@
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7560,10 +7611,10 @@
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -7577,10 +7628,10 @@
       <c r="A2" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="2" t="s">
         <v>265</v>
       </c>
     </row>
@@ -7588,10 +7639,10 @@
       <c r="A3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="2" t="s">
         <v>267</v>
       </c>
     </row>
@@ -7599,10 +7650,10 @@
       <c r="A4" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="2" t="s">
         <v>269</v>
       </c>
     </row>
@@ -7610,7 +7661,7 @@
       <c r="A5" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -7618,7 +7669,7 @@
       <c r="A6" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="2" t="s">
         <v>271</v>
       </c>
     </row>
@@ -7634,7 +7685,7 @@
       <c r="A8" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -7642,7 +7693,7 @@
       <c r="A9" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="2" t="s">
         <v>274</v>
       </c>
     </row>
@@ -7650,7 +7701,7 @@
       <c r="A10" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="2" t="s">
         <v>275</v>
       </c>
     </row>
@@ -7658,7 +7709,7 @@
       <c r="A11" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="2" t="s">
         <v>276</v>
       </c>
     </row>
@@ -7666,7 +7717,7 @@
       <c r="A12" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="2" t="s">
         <v>277</v>
       </c>
     </row>
@@ -7674,7 +7725,7 @@
       <c r="A13" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="2" t="s">
         <v>278</v>
       </c>
     </row>
@@ -7682,7 +7733,7 @@
       <c r="A14" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="2" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7690,7 +7741,7 @@
       <c r="A15" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="2" t="s">
         <v>280</v>
       </c>
     </row>
@@ -7698,7 +7749,7 @@
       <c r="A16" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="2" t="s">
         <v>281</v>
       </c>
     </row>
@@ -7706,7 +7757,7 @@
       <c r="A17" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="2" t="s">
         <v>282</v>
       </c>
     </row>
@@ -7714,7 +7765,7 @@
       <c r="A18" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="2" t="s">
         <v>283</v>
       </c>
     </row>
@@ -7722,7 +7773,7 @@
       <c r="A19" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="2" t="s">
         <v>284</v>
       </c>
     </row>
@@ -7730,7 +7781,7 @@
       <c r="A20" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="2" t="s">
         <v>285</v>
       </c>
     </row>
@@ -7738,7 +7789,7 @@
       <c r="A21" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="2" t="s">
         <v>286</v>
       </c>
     </row>
@@ -7746,7 +7797,7 @@
       <c r="A22" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="2" t="s">
         <v>287</v>
       </c>
     </row>
@@ -7815,10 +7866,10 @@
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -7829,7 +7880,7 @@
       <c r="A2" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>293</v>
       </c>
     </row>
@@ -7837,7 +7888,7 @@
       <c r="A3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>294</v>
       </c>
     </row>
@@ -7845,7 +7896,7 @@
       <c r="A4" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>295</v>
       </c>
     </row>
@@ -7853,7 +7904,7 @@
       <c r="A5" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>296</v>
       </c>
     </row>
@@ -7861,7 +7912,7 @@
       <c r="A6" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>297</v>
       </c>
     </row>
@@ -7869,7 +7920,7 @@
       <c r="A7" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>298</v>
       </c>
     </row>
@@ -7877,7 +7928,7 @@
       <c r="A8" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>299</v>
       </c>
     </row>
@@ -7885,7 +7936,7 @@
       <c r="A9" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>300</v>
       </c>
     </row>
@@ -7893,7 +7944,7 @@
       <c r="A10" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>301</v>
       </c>
     </row>
@@ -7901,7 +7952,7 @@
       <c r="A11" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>302</v>
       </c>
     </row>
@@ -7909,7 +7960,7 @@
       <c r="A12" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>303</v>
       </c>
     </row>
@@ -7917,7 +7968,7 @@
       <c r="A13" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>304</v>
       </c>
     </row>
@@ -7925,7 +7976,7 @@
       <c r="A14" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>305</v>
       </c>
     </row>
@@ -7933,7 +7984,7 @@
       <c r="A15" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>306</v>
       </c>
     </row>
@@ -7941,7 +7992,7 @@
       <c r="A16" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>307</v>
       </c>
     </row>
@@ -7949,7 +8000,7 @@
       <c r="A17" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>308</v>
       </c>
     </row>
@@ -7957,7 +8008,7 @@
       <c r="A18" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>309</v>
       </c>
     </row>
@@ -7965,7 +8016,7 @@
       <c r="A19" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7973,7 +8024,7 @@
       <c r="A20" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>311</v>
       </c>
     </row>
@@ -7981,7 +8032,7 @@
       <c r="A21" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>312</v>
       </c>
     </row>
@@ -7989,7 +8040,7 @@
       <c r="A22" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>313</v>
       </c>
     </row>
@@ -7997,7 +8048,7 @@
       <c r="A23" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>314</v>
       </c>
     </row>
@@ -8005,7 +8056,7 @@
       <c r="A24" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>315</v>
       </c>
     </row>
@@ -8013,7 +8064,7 @@
       <c r="A25" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>316</v>
       </c>
     </row>
@@ -8021,7 +8072,7 @@
       <c r="A26" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>317</v>
       </c>
     </row>
@@ -8029,7 +8080,7 @@
       <c r="A27" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>318</v>
       </c>
     </row>
@@ -8049,7 +8100,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -8058,687 +8109,138 @@
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A1" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>352</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>364</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>373</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>383</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>391</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>400</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>406</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>409</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>414</v>
+        <v>329</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>421</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>427</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>433</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>447</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>450</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>459</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>461</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>476</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>484</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>486</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>488</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>290</v>
+        <v>340</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>493</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -8757,7 +8259,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -8767,10 +8269,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>494</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>495</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8778,13 +8280,40 @@
         <v>186</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>496</v>
+        <v>343</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>293</v>
+        <v>344</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8792,42 +8321,156 @@
         <v>189</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>294</v>
+        <v>355</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>295</v>
+      <c r="B4" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>296</v>
+      <c r="B5" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>297</v>
+      <c r="B6" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>298</v>
+      <c r="B7" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8835,21 +8478,63 @@
         <v>204</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>299</v>
+        <v>398</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>500</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>300</v>
+      <c r="B9" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8857,10 +8542,40 @@
         <v>210</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>301</v>
+        <v>416</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8868,18 +8583,30 @@
         <v>213</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>302</v>
+        <v>427</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>303</v>
+      <c r="B12" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8887,16 +8614,19 @@
         <v>219</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>503</v>
+        <v>434</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>504</v>
+        <v>435</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>304</v>
+        <v>436</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8904,13 +8634,25 @@
         <v>222</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>506</v>
+        <v>439</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>305</v>
+        <v>440</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8918,10 +8660,22 @@
         <v>225</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>306</v>
+        <v>446</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8929,22 +8683,22 @@
         <v>228</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>509</v>
+        <v>452</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>510</v>
+        <v>453</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>307</v>
+        <v>454</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>455</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>513</v>
+        <v>456</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8952,31 +8706,46 @@
         <v>231</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>514</v>
+        <v>458</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>515</v>
+        <v>459</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>516</v>
+        <v>460</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>517</v>
+        <v>461</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>518</v>
+        <v>462</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>519</v>
+        <v>463</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>520</v>
+        <v>464</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>308</v>
+        <v>465</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8984,7 +8753,13 @@
         <v>234</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>309</v>
+        <v>472</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8992,10 +8767,37 @@
         <v>237</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>310</v>
+        <v>475</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9003,40 +8805,49 @@
         <v>239</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>523</v>
+        <v>486</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>524</v>
+        <v>487</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>525</v>
+        <v>488</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>526</v>
+        <v>489</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>311</v>
+        <v>490</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>491</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>528</v>
+        <v>492</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>529</v>
+        <v>493</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>531</v>
+        <v>494</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>495</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>532</v>
+        <v>496</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>533</v>
+        <v>497</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9044,13 +8855,31 @@
         <v>242</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>534</v>
+        <v>286</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>312</v>
+        <v>501</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9058,13 +8887,10 @@
         <v>245</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>313</v>
+        <v>509</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9072,10 +8898,13 @@
         <v>248</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>314</v>
+        <v>288</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9083,10 +8912,16 @@
         <v>251</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>315</v>
+        <v>513</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9094,26 +8929,26 @@
         <v>254</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>316</v>
+        <v>516</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>317</v>
+      <c r="B26" s="8" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>318</v>
+      <c r="B27" s="8" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -9132,6 +8967,381 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -9142,27 +9352,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>541</v>
+        <v>565</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>542</v>
+        <v>566</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>543</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>544</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>545</v>
+        <v>569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>